<commit_message>
See what this looks like
</commit_message>
<xml_diff>
--- a/FamilyLeague.xlsx
+++ b/FamilyLeague.xlsx
@@ -1218,7 +1218,7 @@
         <v>4.333333333333333</v>
       </c>
       <c r="D2">
-        <v>48</v>
+        <v>0.333333333333333</v>
       </c>
       <c r="E2" t="s">
         <v>13</v>
@@ -1235,7 +1235,7 @@
         <v>4.25</v>
       </c>
       <c r="D3">
-        <v>47</v>
+        <v>0.25</v>
       </c>
       <c r="E3" t="s">
         <v>13</v>
@@ -1252,7 +1252,7 @@
         <v>4</v>
       </c>
       <c r="D4">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="E4" t="s">
         <v>13</v>
@@ -1269,7 +1269,7 @@
         <v>3.666666666666667</v>
       </c>
       <c r="D5">
-        <v>39</v>
+        <v>-1.333333333333333</v>
       </c>
       <c r="E5" t="s">
         <v>18</v>
@@ -1286,7 +1286,7 @@
         <v>3.5</v>
       </c>
       <c r="D6">
-        <v>38</v>
+        <v>-0.5</v>
       </c>
       <c r="E6" t="s">
         <v>13</v>
@@ -1303,7 +1303,7 @@
         <v>3.333333333333333</v>
       </c>
       <c r="D7">
-        <v>37</v>
+        <v>0.3333333333333335</v>
       </c>
       <c r="E7" t="s">
         <v>17</v>
@@ -1320,7 +1320,7 @@
         <v>2.916666666666667</v>
       </c>
       <c r="D8">
-        <v>32</v>
+        <v>-0.08333333333333348</v>
       </c>
       <c r="E8" t="s">
         <v>17</v>
@@ -1337,7 +1337,7 @@
         <v>2.916666666666667</v>
       </c>
       <c r="D9">
-        <v>34</v>
+        <v>1.916666666666667</v>
       </c>
       <c r="E9" t="s">
         <v>15</v>
@@ -1354,7 +1354,7 @@
         <v>2.666666666666667</v>
       </c>
       <c r="D10">
-        <v>29</v>
+        <v>-0.3333333333333335</v>
       </c>
       <c r="E10" t="s">
         <v>17</v>
@@ -1371,7 +1371,7 @@
         <v>2.083333333333333</v>
       </c>
       <c r="D11">
-        <v>22</v>
+        <v>-0.9166666666666665</v>
       </c>
       <c r="E11" t="s">
         <v>17</v>
@@ -1388,7 +1388,7 @@
         <v>1.416666666666667</v>
       </c>
       <c r="D12">
-        <v>16</v>
+        <v>0.4166666666666667</v>
       </c>
       <c r="E12" t="s">
         <v>15</v>
@@ -1405,7 +1405,7 @@
         <v>0.9166666666666666</v>
       </c>
       <c r="D13">
-        <v>10</v>
+        <v>-0.08333333333333337</v>
       </c>
       <c r="E13" t="s">
         <v>15</v>

</xml_diff>